<commit_message>
changed version a bit
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1b_CO2_Fluid_Inclusions/PseudoVoigt.xlsx
+++ b/docs/Examples/Example1b_CO2_Fluid_Inclusions/PseudoVoigt.xlsx
@@ -700,61 +700,61 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>0.9978598860796123</v>
+        <v>0.997864610145206</v>
       </c>
       <c r="D2">
-        <v>3.987360630922584E-05</v>
+        <v>4.03400576448685E-05</v>
       </c>
       <c r="E2">
-        <v>331.1864109950466</v>
+        <v>331.1848431006515</v>
       </c>
       <c r="F2">
-        <v>1447.507791711392</v>
+        <v>1447.507791857052</v>
       </c>
       <c r="G2">
-        <v>1116.321380716346</v>
+        <v>1116.3229487564</v>
       </c>
       <c r="H2">
-        <v>49150.03938907994</v>
+        <v>49150.05459653677</v>
       </c>
       <c r="I2">
-        <v>4064.558187157941</v>
+        <v>4103.130676205455</v>
       </c>
       <c r="J2">
-        <v>122.7893778732266</v>
+        <v>122.7899562924199</v>
       </c>
       <c r="K2">
-        <v>11.05666432640984</v>
+        <v>11.33966805013822</v>
       </c>
       <c r="L2">
-        <v>3.987360630922584E-05</v>
+        <v>4.03400576448685E-05</v>
       </c>
       <c r="M2">
-        <v>0.3831035754123102</v>
+        <v>0.3831039430169797</v>
       </c>
       <c r="O2">
-        <v>0.00257</v>
+        <v>0.00258</v>
       </c>
       <c r="P2">
-        <v>0.405291536749454</v>
+        <v>0.4052909952313641</v>
       </c>
       <c r="Q2">
-        <v>0.4051926376392343</v>
+        <v>0.4016441217882361</v>
       </c>
       <c r="S2">
-        <v>0.01295310312974792</v>
+        <v>0.01310853227799338</v>
       </c>
       <c r="T2">
-        <v>0.2777918959532876</v>
+        <v>0.3142723187782764</v>
       </c>
       <c r="U2">
-        <v>0.9978131173855738</v>
+        <v>0.9978173426149631</v>
       </c>
       <c r="V2">
-        <v>0.9979066591580656</v>
+        <v>0.9979118821538743</v>
       </c>
       <c r="W2">
-        <v>133.8460421996364</v>
+        <v>134.1296243425581</v>
       </c>
       <c r="X2" t="s">
         <v>44</v>
@@ -770,6 +770,9 @@
       </c>
       <c r="AB2">
         <v>28</v>
+      </c>
+      <c r="AC2">
+        <v>11.978</v>
       </c>
       <c r="AD2">
         <v>45</v>
@@ -801,61 +804,61 @@
         <v>36</v>
       </c>
       <c r="C3">
-        <v>0.9978264842220211</v>
+        <v>0.9978292451472734</v>
       </c>
       <c r="D3">
-        <v>3.57430383875218E-05</v>
+        <v>3.583090569095404E-05</v>
       </c>
       <c r="E3">
-        <v>331.1974973327126</v>
+        <v>331.1965809318972</v>
       </c>
       <c r="F3">
-        <v>1447.503005381121</v>
+        <v>1447.503005802524</v>
       </c>
       <c r="G3">
-        <v>1116.305508048408</v>
+        <v>1116.306424870626</v>
       </c>
       <c r="H3">
-        <v>48194.63294913297</v>
+        <v>48194.59125163723</v>
       </c>
       <c r="I3">
-        <v>4249.843322072755</v>
+        <v>4256.947837843626</v>
       </c>
       <c r="J3">
-        <v>113.0786756227321</v>
+        <v>113.0789815084083</v>
       </c>
       <c r="K3">
-        <v>9.905378667281072</v>
+        <v>11.09199890916404</v>
       </c>
       <c r="L3">
-        <v>3.57430383875218E-05</v>
+        <v>3.583090569095404E-05</v>
       </c>
       <c r="M3">
-        <v>0.3857421092605332</v>
+        <v>0.3857432425476348</v>
       </c>
       <c r="O3">
         <v>0.0024</v>
       </c>
       <c r="P3">
-        <v>0.3997918883762511</v>
+        <v>0.399786534923933</v>
       </c>
       <c r="Q3">
-        <v>0.4092017687249572</v>
+        <v>0.4074675873316524</v>
       </c>
       <c r="S3">
-        <v>0.01159216800643426</v>
+        <v>0.01162185150579935</v>
       </c>
       <c r="T3">
-        <v>0.2893279115707663</v>
+        <v>0.3016542752120749</v>
       </c>
       <c r="U3">
-        <v>0.9977843306245427</v>
+        <v>0.9977870018936271</v>
       </c>
       <c r="V3">
-        <v>0.9978686413813932</v>
+        <v>0.997871491977972</v>
       </c>
       <c r="W3">
-        <v>122.9840542900132</v>
+        <v>124.1709804175723</v>
       </c>
       <c r="X3" t="s">
         <v>45</v>
@@ -871,6 +874,9 @@
       </c>
       <c r="AB3">
         <v>28</v>
+      </c>
+      <c r="AC3">
+        <v>12.08</v>
       </c>
       <c r="AD3">
         <v>45</v>
@@ -902,61 +908,61 @@
         <v>37</v>
       </c>
       <c r="C4">
-        <v>0.9978100509622898</v>
+        <v>0.9978095733888616</v>
       </c>
       <c r="D4">
-        <v>3.933335809059285E-05</v>
+        <v>3.906085247667861E-05</v>
       </c>
       <c r="E4">
-        <v>331.2029519325042</v>
+        <v>331.2031104534619</v>
       </c>
       <c r="F4">
-        <v>1447.521962191433</v>
+        <v>1447.521962537725</v>
       </c>
       <c r="G4">
-        <v>1116.319010258929</v>
+        <v>1116.318852084263</v>
       </c>
       <c r="H4">
-        <v>46080.58188972915</v>
+        <v>46080.55311799021</v>
       </c>
       <c r="I4">
-        <v>3842.899468127829</v>
+        <v>3817.579597394361</v>
       </c>
       <c r="J4">
-        <v>109.3326919313476</v>
+        <v>109.3331012484569</v>
       </c>
       <c r="K4">
-        <v>10.20425453009774</v>
+        <v>11.0728536290639</v>
       </c>
       <c r="L4">
-        <v>3.933335809059284E-05</v>
+        <v>3.906085247667862E-05</v>
       </c>
       <c r="M4">
-        <v>0.3896353958047211</v>
+        <v>0.3896362373277412</v>
       </c>
       <c r="O4">
         <v>0.00243</v>
       </c>
       <c r="P4">
-        <v>0.4037278540818179</v>
+        <v>0.4037236656929212</v>
       </c>
       <c r="Q4">
-        <v>0.406028126976008</v>
+        <v>0.4066422061589337</v>
       </c>
       <c r="S4">
-        <v>0.01279868269207621</v>
+        <v>0.01270681042663709</v>
       </c>
       <c r="T4">
-        <v>0.2818591713753829</v>
+        <v>0.2643135192520635</v>
       </c>
       <c r="U4">
-        <v>0.9977641738530534</v>
+        <v>0.9977639730800651</v>
       </c>
       <c r="V4">
-        <v>0.997855932290571</v>
+        <v>0.9978551778659448</v>
       </c>
       <c r="W4">
-        <v>119.5369464614454</v>
+        <v>120.4059548775208</v>
       </c>
       <c r="X4" t="s">
         <v>46</v>
@@ -972,6 +978,9 @@
       </c>
       <c r="AB4">
         <v>28</v>
+      </c>
+      <c r="AC4">
+        <v>19.977</v>
       </c>
       <c r="AD4">
         <v>45</v>
@@ -1003,61 +1012,61 @@
         <v>38</v>
       </c>
       <c r="C5">
-        <v>0.9977826198315888</v>
+        <v>0.9977819301559424</v>
       </c>
       <c r="D5">
-        <v>4.053693854759805E-05</v>
+        <v>4.021169415392708E-05</v>
       </c>
       <c r="E5">
-        <v>331.2120573942375</v>
+        <v>331.2122863309248</v>
       </c>
       <c r="F5">
-        <v>1447.539256518417</v>
+        <v>1447.539256706479</v>
       </c>
       <c r="G5">
-        <v>1116.32719912418</v>
+        <v>1116.326970375554</v>
       </c>
       <c r="H5">
-        <v>44440.9420876005</v>
+        <v>44440.93230787192</v>
       </c>
       <c r="I5">
-        <v>3811.741538002881</v>
+        <v>3778.687317392505</v>
       </c>
       <c r="J5">
-        <v>106.9637865077495</v>
+        <v>106.9642679490747</v>
       </c>
       <c r="K5">
-        <v>10.36403580892033</v>
+        <v>11.41406198750633</v>
       </c>
       <c r="L5">
-        <v>4.053693854759805E-05</v>
+        <v>4.021169415392707E-05</v>
       </c>
       <c r="M5">
-        <v>0.3914122320374968</v>
+        <v>0.3914127086273933</v>
       </c>
       <c r="O5">
         <v>0.00242</v>
       </c>
       <c r="P5">
-        <v>0.4092346608981216</v>
+        <v>0.4092324959144185</v>
       </c>
       <c r="Q5">
-        <v>0.4082686204520876</v>
+        <v>0.4091641516886602</v>
       </c>
       <c r="S5">
-        <v>0.0132064281462208</v>
+        <v>0.0130969040856272</v>
       </c>
       <c r="T5">
-        <v>0.2859551890075377</v>
+        <v>0.2628163049414113</v>
       </c>
       <c r="U5">
-        <v>0.997735547140579</v>
+        <v>0.9977351874418423</v>
       </c>
       <c r="V5">
-        <v>0.9978296969645427</v>
+        <v>0.9978286772499295</v>
       </c>
       <c r="W5">
-        <v>117.3278223166699</v>
+        <v>118.378329936581</v>
       </c>
       <c r="X5" t="s">
         <v>47</v>
@@ -1073,6 +1082,9 @@
       </c>
       <c r="AB5">
         <v>28</v>
+      </c>
+      <c r="AC5">
+        <v>12.044</v>
       </c>
       <c r="AD5">
         <v>45</v>
@@ -1104,61 +1116,61 @@
         <v>39</v>
       </c>
       <c r="C6">
-        <v>0.9977781961827885</v>
+        <v>0.9977783725275983</v>
       </c>
       <c r="D6">
-        <v>3.799534336316177E-05</v>
+        <v>3.762356284133659E-05</v>
       </c>
       <c r="E6">
-        <v>331.2135258226176</v>
+        <v>331.2134672847822</v>
       </c>
       <c r="F6">
-        <v>1447.541011877257</v>
+        <v>1447.541012035804</v>
       </c>
       <c r="G6">
-        <v>1116.32748605464</v>
+        <v>1116.327544751022</v>
       </c>
       <c r="H6">
-        <v>45288.66855610132</v>
+        <v>45288.66273637601</v>
       </c>
       <c r="I6">
-        <v>3947.474007742397</v>
+        <v>3904.517386088566</v>
       </c>
       <c r="J6">
-        <v>110.8975282102296</v>
+        <v>110.8980180547772</v>
       </c>
       <c r="K6">
-        <v>10.91844694552933</v>
+        <v>12.56714227142768</v>
       </c>
       <c r="L6">
-        <v>3.799534336316177E-05</v>
+        <v>3.762356284133659E-05</v>
       </c>
       <c r="M6">
-        <v>0.3933158774344163</v>
+        <v>0.3933162854106986</v>
       </c>
       <c r="O6">
         <v>0.00251</v>
       </c>
       <c r="P6">
-        <v>0.4163762948292194</v>
+        <v>0.4163746000991697</v>
       </c>
       <c r="Q6">
-        <v>0.4098356067117886</v>
+        <v>0.4102546201380286</v>
       </c>
       <c r="S6">
-        <v>0.01233172102207001</v>
+        <v>0.01220602945670827</v>
       </c>
       <c r="T6">
-        <v>0.2926682750136492</v>
+        <v>0.2668567001166197</v>
       </c>
       <c r="U6">
-        <v>0.997733487615888</v>
+        <v>0.9977340425561128</v>
       </c>
       <c r="V6">
-        <v>0.9978229087566619</v>
+        <v>0.9978227064384776</v>
       </c>
       <c r="W6">
-        <v>121.8159751557589</v>
+        <v>123.4651603262049</v>
       </c>
       <c r="X6" t="s">
         <v>48</v>
@@ -1174,6 +1186,9 @@
       </c>
       <c r="AB6">
         <v>28</v>
+      </c>
+      <c r="AC6">
+        <v>19.988</v>
       </c>
       <c r="AD6">
         <v>45</v>
@@ -1205,61 +1220,61 @@
         <v>40</v>
       </c>
       <c r="C7">
-        <v>0.997775737608652</v>
+        <v>0.9977801156790581</v>
       </c>
       <c r="D7">
-        <v>3.521989263082476E-05</v>
+        <v>3.554953358906369E-05</v>
       </c>
       <c r="E7">
-        <v>331.2143419509093</v>
+        <v>331.2128886450298</v>
       </c>
       <c r="F7">
-        <v>1447.539632678197</v>
+        <v>1447.539632846651</v>
       </c>
       <c r="G7">
-        <v>1116.325290727288</v>
+        <v>1116.326744201622</v>
       </c>
       <c r="H7">
-        <v>46370.34161343362</v>
+        <v>46370.33402072885</v>
       </c>
       <c r="I7">
-        <v>4254.113932483191</v>
+        <v>4282.108479381145</v>
       </c>
       <c r="J7">
-        <v>116.1392139824934</v>
+        <v>116.1397256563911</v>
       </c>
       <c r="K7">
-        <v>11.1446659173381</v>
+        <v>12.37561484100051</v>
       </c>
       <c r="L7">
-        <v>3.521989263082476E-05</v>
+        <v>3.554953358906369E-05</v>
       </c>
       <c r="M7">
-        <v>0.3925913687643211</v>
+        <v>0.3925918093317671</v>
       </c>
       <c r="O7">
         <v>0.00257</v>
       </c>
       <c r="P7">
-        <v>0.4170039054175857</v>
+        <v>0.4170020136156424</v>
       </c>
       <c r="Q7">
-        <v>0.4046799468193902</v>
+        <v>0.4013845083479939</v>
       </c>
       <c r="S7">
-        <v>0.01137871289278358</v>
+        <v>0.01149056550647157</v>
       </c>
       <c r="T7">
-        <v>0.3126667295924849</v>
+        <v>0.3407948763191531</v>
       </c>
       <c r="U7">
-        <v>0.9977337191951056</v>
+        <v>0.9977377599688388</v>
       </c>
       <c r="V7">
-        <v>0.9978177595614622</v>
+        <v>0.9978224749855779</v>
       </c>
       <c r="W7">
-        <v>127.2838798998315</v>
+        <v>128.5153404973916</v>
       </c>
       <c r="X7" t="s">
         <v>49</v>
@@ -1275,6 +1290,9 @@
       </c>
       <c r="AB7">
         <v>28</v>
+      </c>
+      <c r="AC7">
+        <v>12.039</v>
       </c>
       <c r="AD7">
         <v>45</v>
@@ -1306,61 +1324,61 @@
         <v>41</v>
       </c>
       <c r="C8">
-        <v>0.9977600522180611</v>
+        <v>0.997763519810411</v>
       </c>
       <c r="D8">
-        <v>3.96303108442229E-05</v>
+        <v>3.996281559342204E-05</v>
       </c>
       <c r="E8">
-        <v>331.2195488403927</v>
+        <v>331.2183977315869</v>
       </c>
       <c r="F8">
-        <v>1447.534557918229</v>
+        <v>1447.534558137279</v>
       </c>
       <c r="G8">
-        <v>1116.315009077836</v>
+        <v>1116.316160405692</v>
       </c>
       <c r="H8">
-        <v>44105.49495871713</v>
+        <v>44105.47704015052</v>
       </c>
       <c r="I8">
-        <v>3915.579106580432</v>
+        <v>3941.970379392729</v>
       </c>
       <c r="J8">
-        <v>102.6329463068532</v>
+        <v>102.6333952862651</v>
       </c>
       <c r="K8">
-        <v>11.22393506653637</v>
+        <v>11.52098883377944</v>
       </c>
       <c r="L8">
-        <v>3.96303108442229E-05</v>
+        <v>3.996281559342204E-05</v>
       </c>
       <c r="M8">
-        <v>0.3949879254397151</v>
+        <v>0.3949885259756325</v>
       </c>
       <c r="O8">
         <v>0.00236</v>
       </c>
       <c r="P8">
-        <v>0.4058043278678481</v>
+        <v>0.4058012811822291</v>
       </c>
       <c r="Q8">
-        <v>0.4070156761523468</v>
+        <v>0.4044871219574797</v>
       </c>
       <c r="S8">
-        <v>0.01291243725375591</v>
+        <v>0.01302433137593426</v>
       </c>
       <c r="T8">
-        <v>0.3022478161670795</v>
+        <v>0.3286078745419824</v>
       </c>
       <c r="U8">
-        <v>0.9977140479129187</v>
+        <v>0.9977171781464422</v>
       </c>
       <c r="V8">
-        <v>0.9978060607658893</v>
+        <v>0.9978098657795067</v>
       </c>
       <c r="W8">
-        <v>113.8568813733896</v>
+        <v>114.1543841200446</v>
       </c>
       <c r="X8" t="s">
         <v>50</v>
@@ -1376,6 +1394,9 @@
       </c>
       <c r="AB8">
         <v>28</v>
+      </c>
+      <c r="AC8">
+        <v>12.059</v>
       </c>
       <c r="AD8">
         <v>45</v>
@@ -1407,61 +1428,61 @@
         <v>42</v>
       </c>
       <c r="C9">
-        <v>0.9977557132171323</v>
+        <v>0.9977587176510911</v>
       </c>
       <c r="D9">
-        <v>4.08649213211015E-05</v>
+        <v>4.11619038602536E-05</v>
       </c>
       <c r="E9">
-        <v>331.2209892349813</v>
+        <v>331.2199918680124</v>
       </c>
       <c r="F9">
-        <v>1447.516894431486</v>
+        <v>1447.516894809508</v>
       </c>
       <c r="G9">
-        <v>1116.295905196504</v>
+        <v>1116.296902941496</v>
       </c>
       <c r="H9">
-        <v>43261.39606674626</v>
+        <v>43261.36597323853</v>
       </c>
       <c r="I9">
-        <v>3835.072595910358</v>
+        <v>3858.442438382513</v>
       </c>
       <c r="J9">
-        <v>108.0927717612777</v>
+        <v>108.0931650600248</v>
       </c>
       <c r="K9">
-        <v>11.09514505542197</v>
+        <v>11.88368840996711</v>
       </c>
       <c r="L9">
-        <v>4.08649213211015E-05</v>
+        <v>4.11619038602536E-05</v>
       </c>
       <c r="M9">
-        <v>0.3929697387808552</v>
+        <v>0.392970700582273</v>
       </c>
       <c r="O9">
         <v>0.00257</v>
       </c>
       <c r="P9">
-        <v>0.4140404255556192</v>
+        <v>0.4140357776661653</v>
       </c>
       <c r="Q9">
-        <v>0.4073028395439339</v>
+        <v>0.4052672146144209</v>
       </c>
       <c r="S9">
-        <v>0.01328909246086156</v>
+        <v>0.01338922658632062</v>
       </c>
       <c r="T9">
-        <v>0.3142053281481823</v>
+        <v>0.3383168108910171</v>
       </c>
       <c r="U9">
-        <v>0.9977079422635405</v>
+        <v>0.9977106447972814</v>
       </c>
       <c r="V9">
-        <v>0.9978034887455564</v>
+        <v>0.9978067951377283</v>
       </c>
       <c r="W9">
-        <v>119.1879168166997</v>
+        <v>119.9768534699919</v>
       </c>
       <c r="X9" t="s">
         <v>51</v>
@@ -1477,6 +1498,9 @@
       </c>
       <c r="AB9">
         <v>28</v>
+      </c>
+      <c r="AC9">
+        <v>12.094</v>
       </c>
       <c r="AD9">
         <v>45</v>
@@ -1508,61 +1532,61 @@
         <v>43</v>
       </c>
       <c r="C10">
-        <v>0.9977568843223</v>
+        <v>0.9977601746701813</v>
       </c>
       <c r="D10">
-        <v>4.065606820687621E-05</v>
+        <v>4.086339614387934E-05</v>
       </c>
       <c r="E10">
-        <v>331.2206004683205</v>
+        <v>331.2195081908087</v>
       </c>
       <c r="F10">
-        <v>1447.524736945334</v>
+        <v>1447.52473729567</v>
       </c>
       <c r="G10">
-        <v>1116.304136477014</v>
+        <v>1116.305229104861</v>
       </c>
       <c r="H10">
-        <v>43156.99290066765</v>
+        <v>43156.96590535386</v>
       </c>
       <c r="I10">
-        <v>3790.648654420056</v>
+        <v>3811.220077453418</v>
       </c>
       <c r="J10">
-        <v>103.7940358126246</v>
+        <v>103.7944535080573</v>
       </c>
       <c r="K10">
-        <v>11.52920847606356</v>
+        <v>12.61453751755598</v>
       </c>
       <c r="L10">
-        <v>4.065606820687622E-05</v>
+        <v>4.086339614387934E-05</v>
       </c>
       <c r="M10">
-        <v>0.3925621523975833</v>
+        <v>0.3925630102433947</v>
       </c>
       <c r="O10">
         <v>0.00244</v>
       </c>
       <c r="P10">
-        <v>0.4168855850620845</v>
+        <v>0.4168813180695979</v>
       </c>
       <c r="Q10">
-        <v>0.4084576872680725</v>
+        <v>0.4062179138014888</v>
       </c>
       <c r="S10">
-        <v>0.01324322412067986</v>
+        <v>0.01331299985468358</v>
       </c>
       <c r="T10">
-        <v>0.3084446521308241</v>
+        <v>0.3314984253568839</v>
       </c>
       <c r="U10">
-        <v>0.9977096429855106</v>
+        <v>0.9977127228504987</v>
       </c>
       <c r="V10">
-        <v>0.9978041301330356</v>
+        <v>0.9978076310037529</v>
       </c>
       <c r="W10">
-        <v>115.3232442886881</v>
+        <v>116.4089910256133</v>
       </c>
       <c r="X10" t="s">
         <v>52</v>
@@ -1578,6 +1602,9 @@
       </c>
       <c r="AB10">
         <v>28</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
       </c>
       <c r="AD10">
         <v>45</v>

</xml_diff>